<commit_message>
KDT_DDT for modification non individual
</commit_message>
<xml_diff>
--- a/DDT.xlsx
+++ b/DDT.xlsx
@@ -3,17 +3,19 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF22014D-3273-4E35-A4BA-D86EC2EDBE71}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63C33B15-3E35-4564-A87B-20BCD4F792A9}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
-    <sheet name="MembershipRegistration" sheetId="2" r:id="rId2"/>
+    <sheet name="MemRegIndividual" sheetId="2" r:id="rId2"/>
     <sheet name="MembRegNonInd" sheetId="4" r:id="rId3"/>
-    <sheet name="transactionEntry" sheetId="7" r:id="rId4"/>
-    <sheet name="CreateFdSingle" sheetId="3" r:id="rId5"/>
-    <sheet name="CreateFdJoint" sheetId="5" r:id="rId6"/>
+    <sheet name="ModNonIndiv" sheetId="8" r:id="rId4"/>
+    <sheet name="transactionEntry" sheetId="7" r:id="rId5"/>
+    <sheet name="ViewFd" sheetId="6" r:id="rId6"/>
+    <sheet name="CreateFdSingle" sheetId="3" r:id="rId7"/>
+    <sheet name="CreateFdJoint" sheetId="5" r:id="rId8"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="121">
   <si>
     <t>beta10</t>
   </si>
@@ -123,40 +125,271 @@
     <t>DEF</t>
   </si>
   <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>ABCD123456</t>
+  </si>
+  <si>
+    <t>panNum</t>
+  </si>
+  <si>
+    <t>89324324324</t>
+  </si>
+  <si>
+    <t>voterID</t>
+  </si>
+  <si>
+    <t>ABCD0123DEFG1234</t>
+  </si>
+  <si>
+    <t>driving</t>
+  </si>
+  <si>
+    <t>passport</t>
+  </si>
+  <si>
+    <t>PQ123456</t>
+  </si>
+  <si>
+    <t>123489073453</t>
+  </si>
+  <si>
+    <t>aadhar</t>
+  </si>
+  <si>
+    <t>xyz colony, m nagar</t>
+  </si>
+  <si>
+    <t>address1</t>
+  </si>
+  <si>
+    <t>Uttar Pradesh</t>
+  </si>
+  <si>
+    <t>address2</t>
+  </si>
+  <si>
+    <t>Mahape</t>
+  </si>
+  <si>
+    <t>village</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>landline</t>
+  </si>
+  <si>
+    <t>mobile</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>income</t>
+  </si>
+  <si>
+    <t>education</t>
+  </si>
+  <si>
+    <t>maritalStatus</t>
+  </si>
+  <si>
+    <t>natureActivity</t>
+  </si>
+  <si>
+    <t>60708901111</t>
+  </si>
+  <si>
+    <t>9897866612</t>
+  </si>
+  <si>
+    <t>harsh.mathur04@gmail.com</t>
+  </si>
+  <si>
+    <t>Graduated</t>
+  </si>
+  <si>
+    <t>Unmarried</t>
+  </si>
+  <si>
+    <t>Others</t>
+  </si>
+  <si>
+    <t>accNum</t>
+  </si>
+  <si>
+    <t>120301 - Harsh Mathur</t>
+  </si>
+  <si>
+    <t>imagePhoto</t>
+  </si>
+  <si>
+    <t>imageSig</t>
+  </si>
+  <si>
+    <t>notification</t>
+  </si>
+  <si>
+    <t>Member Registered successfully</t>
+  </si>
+  <si>
+    <t>pinNum</t>
+  </si>
+  <si>
+    <t>120403-Kanika Kapish</t>
+  </si>
+  <si>
+    <t>member</t>
+  </si>
+  <si>
+    <t>D:\\SoftPAC\\SoftPAC_v4\\SoftPAC\\SoftPACTesting\\test\\resources\\data\\images\\photo.png</t>
+  </si>
+  <si>
+    <t>D:\\SoftPAC\\SoftPAC_v4\\SoftPAC\\SoftPACTesting\\test\\resources\\data\\images\\sign.png</t>
+  </si>
+  <si>
     <t>memberId</t>
   </si>
   <si>
+    <t>accountNo</t>
+  </si>
+  <si>
+    <t>transactionType</t>
+  </si>
+  <si>
+    <t>instrumentType</t>
+  </si>
+  <si>
+    <t>transactionCode</t>
+  </si>
+  <si>
+    <t>amount</t>
+  </si>
+  <si>
     <t>120892-Vikash Anand .</t>
   </si>
   <si>
     <t>CA 742-Vikash Anand .</t>
   </si>
   <si>
-    <t>accountNo</t>
-  </si>
-  <si>
-    <t>instrumentType</t>
+    <t>Credit</t>
   </si>
   <si>
     <t>Withdrawal Slip</t>
   </si>
   <si>
-    <t>transactionType</t>
-  </si>
-  <si>
     <t>CA</t>
   </si>
   <si>
-    <t>amount</t>
-  </si>
-  <si>
-    <t>Credit</t>
-  </si>
-  <si>
     <t>Debit</t>
   </si>
   <si>
-    <t>transactionCode</t>
+    <t>action</t>
+  </si>
+  <si>
+    <t>Modify</t>
+  </si>
+  <si>
+    <t>constitution</t>
+  </si>
+  <si>
+    <t>Partnership</t>
+  </si>
+  <si>
+    <t>docDetails</t>
+  </si>
+  <si>
+    <t>important docs</t>
+  </si>
+  <si>
+    <t>docName</t>
+  </si>
+  <si>
+    <t>Passport</t>
+  </si>
+  <si>
+    <t>docAuth</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>docIssue</t>
+  </si>
+  <si>
+    <t>Delhi</t>
+  </si>
+  <si>
+    <t>docNum</t>
+  </si>
+  <si>
+    <t>ABCD1023</t>
+  </si>
+  <si>
+    <t>docDate</t>
+  </si>
+  <si>
+    <t>25-04-2018</t>
+  </si>
+  <si>
+    <t>CNSPM11234</t>
+  </si>
+  <si>
+    <t>pin</t>
+  </si>
+  <si>
+    <t>mob</t>
+  </si>
+  <si>
+    <t xml:space="preserve">income </t>
+  </si>
+  <si>
+    <t>activity</t>
+  </si>
+  <si>
+    <t>photoImg</t>
+  </si>
+  <si>
+    <t>signImg</t>
+  </si>
+  <si>
+    <t>C:\\Users\\LTI.INFVA07202\\Documents\\Workspace\\SoftPAC\\SoftPACTesting\\test\\resources\\data\\images\\sign.png</t>
+  </si>
+  <si>
+    <t>C:\\Users\\LTI.INFVA07202\\Documents\\Workspace\\SoftPAC\\SoftPACTesting\\test\\resources\\data\\images\\photo.png</t>
+  </si>
+  <si>
+    <t>Divice</t>
+  </si>
+  <si>
+    <t>Post Graduated</t>
+  </si>
+  <si>
+    <t>2000000</t>
+  </si>
+  <si>
+    <t>vaisahali.001@gmail.com</t>
+  </si>
+  <si>
+    <t>1234567891</t>
+  </si>
+  <si>
+    <t>12345687977</t>
+  </si>
+  <si>
+    <t>UP</t>
+  </si>
+  <si>
+    <t>LTI</t>
+  </si>
+  <si>
+    <t>mahape</t>
+  </si>
+  <si>
+    <t>thane</t>
   </si>
 </sst>
 </file>
@@ -253,7 +486,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -265,21 +498,41 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -565,7 +818,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -609,32 +862,50 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{514BFD99-4204-4030-86CA-47FBED926B7C}">
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:AI2"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+    <sheetView topLeftCell="Y1" workbookViewId="0">
+      <selection activeCell="Y1" sqref="Y1:Y2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" style="5" customWidth="1"/>
-    <col min="2" max="2" width="17" style="5" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" style="5" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" style="5" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="5"/>
-    <col min="7" max="7" width="10.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13" style="5" customWidth="1"/>
-    <col min="9" max="9" width="18.28515625" style="5" customWidth="1"/>
-    <col min="10" max="10" width="13.28515625" style="5" customWidth="1"/>
-    <col min="11" max="11" width="14.5703125" style="5" customWidth="1"/>
-    <col min="12" max="12" width="12.7109375" style="5" customWidth="1"/>
-    <col min="13" max="13" width="17.140625" style="5" customWidth="1"/>
-    <col min="14" max="14" width="16.42578125" style="5" customWidth="1"/>
-    <col min="15" max="16384" width="9.140625" style="5"/>
+    <col min="1" max="1" width="16.5703125" style="6" customWidth="1"/>
+    <col min="2" max="2" width="17" style="6" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" style="6" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" style="6" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="6"/>
+    <col min="7" max="7" width="10.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13" style="6" customWidth="1"/>
+    <col min="9" max="9" width="18.28515625" style="6" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" style="6" customWidth="1"/>
+    <col min="11" max="11" width="14.5703125" style="6" customWidth="1"/>
+    <col min="12" max="12" width="12.7109375" style="6" customWidth="1"/>
+    <col min="13" max="13" width="17.140625" style="6" customWidth="1"/>
+    <col min="14" max="14" width="16.42578125" style="6" customWidth="1"/>
+    <col min="15" max="15" width="13.140625" style="6" customWidth="1"/>
+    <col min="16" max="16" width="13.7109375" style="6" customWidth="1"/>
+    <col min="17" max="17" width="19.28515625" style="6" customWidth="1"/>
+    <col min="18" max="18" width="16.5703125" style="6" customWidth="1"/>
+    <col min="19" max="19" width="15.5703125" style="6" customWidth="1"/>
+    <col min="20" max="20" width="20.85546875" style="6" customWidth="1"/>
+    <col min="21" max="21" width="13.85546875" style="6" customWidth="1"/>
+    <col min="22" max="24" width="9.140625" style="6"/>
+    <col min="25" max="25" width="12.7109375" style="6" customWidth="1"/>
+    <col min="26" max="26" width="13" style="6" customWidth="1"/>
+    <col min="27" max="28" width="9.140625" style="6"/>
+    <col min="29" max="29" width="13.42578125" style="6" customWidth="1"/>
+    <col min="30" max="30" width="14.140625" style="6" customWidth="1"/>
+    <col min="31" max="31" width="14.42578125" style="6" customWidth="1"/>
+    <col min="32" max="32" width="27.7109375" style="6" customWidth="1"/>
+    <col min="33" max="33" width="31.5703125" style="6" customWidth="1"/>
+    <col min="34" max="34" width="23" style="6" customWidth="1"/>
+    <col min="35" max="35" width="17" style="6" customWidth="1"/>
+    <col min="36" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -677,47 +948,173 @@
       <c r="N1" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="O1" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="S1" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="T1" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="U1" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="V1" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="W1" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="X1" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="Y1" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Z1" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AA1" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AB1" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AC1" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AD1" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AE1" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF1" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="AG1" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="AH1" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="AI1" s="5" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="2" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:35" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6" t="s">
+      <c r="D2" s="7"/>
+      <c r="E2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="6">
-        <v>100</v>
-      </c>
-      <c r="K2" s="6" t="s">
+      <c r="J2" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="K2" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="L2" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="M2" s="6" t="s">
+      <c r="M2" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="N2" s="6" t="s">
+      <c r="N2" s="7" t="s">
         <v>31</v>
+      </c>
+      <c r="O2" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="P2" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q2" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="R2" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="S2" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="T2" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="U2" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="V2" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="W2" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="X2" s="9">
+        <v>510011</v>
+      </c>
+      <c r="Y2" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="Z2" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA2" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AB2" s="7">
+        <v>50000</v>
+      </c>
+      <c r="AC2" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AD2" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE2" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="AF2" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="AG2" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="AH2" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="AI2" s="7" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -730,8 +1127,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E61D5CB3-3A90-4B9A-B616-2DE224B83C03}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -741,81 +1138,155 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{668676D6-4BBB-445B-8898-FAACA9269FC4}">
-  <dimension ref="A1:F3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49030D74-C4FA-4736-81C0-ADA3B799FDDE}">
+  <dimension ref="A1:V2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" style="10" customWidth="1"/>
-    <col min="2" max="2" width="24.5703125" style="10" customWidth="1"/>
-    <col min="3" max="3" width="19.5703125" style="10" customWidth="1"/>
-    <col min="4" max="4" width="22.7109375" style="10" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="10"/>
+    <col min="15" max="15" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="23.140625" customWidth="1"/>
+    <col min="21" max="21" width="21.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="B1" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>40</v>
+    <row r="1" spans="1:22" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>108</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="F2" s="8">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="F3" s="10">
-        <v>100</v>
+    <row r="2" spans="1:22" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="K2" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="L2" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="M2" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="N2" s="20">
+        <v>482002</v>
+      </c>
+      <c r="O2" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="P2" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q2" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="R2" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="S2" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="T2" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="U2" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="V2" s="13" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -824,6 +1295,116 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC50F3F2-A7E3-42E2-AFB0-6A6894AB7B7C}">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32.42578125" customWidth="1"/>
+    <col min="2" max="2" width="23.7109375" customWidth="1"/>
+    <col min="3" max="3" width="24.7109375" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" customWidth="1"/>
+    <col min="5" max="5" width="20.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="F2" s="13">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="F3" s="15">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{201A1C50-5B6F-4A9E-89AE-F878864A77B8}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FA1A9CA-CA22-4BB4-A1EA-E24D7DFE4254}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -837,7 +1418,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AFA3F5A-DB7E-4EC3-BC59-81110CB4D302}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>